<commit_message>
probe interface is changed
</commit_message>
<xml_diff>
--- a/alarmData.xlsx
+++ b/alarmData.xlsx
@@ -397,9 +397,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
   <sheetData>
     <row r="1">
@@ -471,9 +471,97 @@
         <v>2024-10-04T10:45:15.524Z</v>
       </c>
     </row>
+    <row r="4">
+      <c r="D4">
+        <v>2</v>
+      </c>
+      <c r="E4" t="str">
+        <v>Heart Rate</v>
+      </c>
+      <c r="F4" t="str">
+        <v>Low</v>
+      </c>
+      <c r="G4" t="str">
+        <v>2024-10-19T12:06:32.829</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="D5">
+        <v>2</v>
+      </c>
+      <c r="E5" t="str">
+        <v>Blood Pressure</v>
+      </c>
+      <c r="F5" t="str">
+        <v>High</v>
+      </c>
+      <c r="G5" t="str">
+        <v>2024-10-19T12:06:33.660</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="D6">
+        <v>2</v>
+      </c>
+      <c r="E6" t="str">
+        <v>Oxygen Saturation</v>
+      </c>
+      <c r="F6" t="str">
+        <v>Very Low</v>
+      </c>
+      <c r="G6" t="str">
+        <v>2024-10-19T12:06:34.831</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="str">
+        <v>2024-10-19</v>
+      </c>
+      <c r="B7" t="str">
+        <v>46</v>
+      </c>
+      <c r="C7" t="str">
+        <v>test3</v>
+      </c>
+      <c r="D7">
+        <v>3</v>
+      </c>
+      <c r="E7" t="str">
+        <v>Heart Rate</v>
+      </c>
+      <c r="F7" t="str">
+        <v>Very Low</v>
+      </c>
+      <c r="G7" t="str">
+        <v>2024-10-19T12:12:04.549</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="str">
+        <v>2024-10-19</v>
+      </c>
+      <c r="B8" t="str">
+        <v>46</v>
+      </c>
+      <c r="C8" t="str">
+        <v>test3</v>
+      </c>
+      <c r="D8">
+        <v>3</v>
+      </c>
+      <c r="E8" t="str">
+        <v>Blood Pressure</v>
+      </c>
+      <c r="F8" t="str">
+        <v>High</v>
+      </c>
+      <c r="G8" t="str">
+        <v>2024-10-19T12:12:05.137</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:G3"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:G8"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
with font size adjustments
</commit_message>
<xml_diff>
--- a/alarmData.xlsx
+++ b/alarmData.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -559,9 +559,78 @@
         <v>2024-10-19T12:12:05.137</v>
       </c>
     </row>
+    <row r="9">
+      <c r="A9" t="str">
+        <v>2024-10-29</v>
+      </c>
+      <c r="B9" t="str">
+        <v>10001</v>
+      </c>
+      <c r="C9" t="str">
+        <v>Khushiremote</v>
+      </c>
+      <c r="D9">
+        <v>4</v>
+      </c>
+      <c r="E9" t="str">
+        <v>Heart Rate</v>
+      </c>
+      <c r="F9" t="str">
+        <v>High</v>
+      </c>
+      <c r="G9" t="str">
+        <v>2024-10-29T14:48:12.956</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="str">
+        <v>2024-10-29</v>
+      </c>
+      <c r="B10" t="str">
+        <v>10001</v>
+      </c>
+      <c r="C10" t="str">
+        <v>Khushiremote</v>
+      </c>
+      <c r="D10">
+        <v>4</v>
+      </c>
+      <c r="E10" t="str">
+        <v>Blood Pressure</v>
+      </c>
+      <c r="F10" t="str">
+        <v>Low</v>
+      </c>
+      <c r="G10" t="str">
+        <v>2024-10-29T14:48:13.605</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="str">
+        <v>2024-10-29</v>
+      </c>
+      <c r="B11" t="str">
+        <v>10001</v>
+      </c>
+      <c r="C11" t="str">
+        <v>Khushiremote</v>
+      </c>
+      <c r="D11">
+        <v>4</v>
+      </c>
+      <c r="E11" t="str">
+        <v>Oxygen Saturation</v>
+      </c>
+      <c r="F11" t="str">
+        <v>Very High</v>
+      </c>
+      <c r="G11" t="str">
+        <v>2024-10-29T14:48:14.571</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:G8"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:G11"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
can now deselect an vital completely and also create separate files for each participant
</commit_message>
<xml_diff>
--- a/alarmData.xlsx
+++ b/alarmData.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -628,9 +628,138 @@
         <v>2024-10-29T14:48:14.571</v>
       </c>
     </row>
+    <row r="12">
+      <c r="D12">
+        <v>5</v>
+      </c>
+      <c r="E12" t="str">
+        <v>Blood Pressure</v>
+      </c>
+      <c r="F12" t="str">
+        <v>Low</v>
+      </c>
+      <c r="G12" t="str">
+        <v>2024-10-30T16:39:38.332</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="str">
+        <v>2024-11-04</v>
+      </c>
+      <c r="B13" t="str">
+        <v>111</v>
+      </c>
+      <c r="C13" t="str">
+        <v>AA111</v>
+      </c>
+      <c r="D13">
+        <v>6</v>
+      </c>
+      <c r="E13" t="str">
+        <v>Blood Pressure</v>
+      </c>
+      <c r="F13" t="str">
+        <v>Very Low</v>
+      </c>
+      <c r="G13" t="str">
+        <v>2024-11-04T06:51:05.800</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="str">
+        <v>2024-11-04</v>
+      </c>
+      <c r="B14" t="str">
+        <v>111</v>
+      </c>
+      <c r="C14" t="str">
+        <v>AA111</v>
+      </c>
+      <c r="D14">
+        <v>7</v>
+      </c>
+      <c r="E14" t="str">
+        <v>Blood Pressure</v>
+      </c>
+      <c r="F14" t="str">
+        <v>Very High</v>
+      </c>
+      <c r="G14" t="str">
+        <v>2024-11-04T06:52:41.859</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="str">
+        <v>2024-11-04</v>
+      </c>
+      <c r="B15" t="str">
+        <v>111</v>
+      </c>
+      <c r="C15" t="str">
+        <v>AA111</v>
+      </c>
+      <c r="D15">
+        <v>7</v>
+      </c>
+      <c r="E15" t="str">
+        <v>Heart Rate</v>
+      </c>
+      <c r="F15" t="str">
+        <v>Static</v>
+      </c>
+      <c r="G15" t="str">
+        <v>2024-11-04T06:52:51.788</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="str">
+        <v>2024-11-04</v>
+      </c>
+      <c r="B16" t="str">
+        <v>112</v>
+      </c>
+      <c r="C16" t="str">
+        <v>AA112</v>
+      </c>
+      <c r="D16">
+        <v>8</v>
+      </c>
+      <c r="E16" t="str">
+        <v>Oxygen Saturation</v>
+      </c>
+      <c r="F16" t="str">
+        <v>High</v>
+      </c>
+      <c r="G16" t="str">
+        <v>2024-11-04T06:57:17.776</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="str">
+        <v>2024-11-04</v>
+      </c>
+      <c r="B17" t="str">
+        <v>113</v>
+      </c>
+      <c r="C17" t="str">
+        <v>Aa1123</v>
+      </c>
+      <c r="D17">
+        <v>9</v>
+      </c>
+      <c r="E17" t="str">
+        <v>Blood Pressure</v>
+      </c>
+      <c r="F17" t="str">
+        <v>Static</v>
+      </c>
+      <c r="G17" t="str">
+        <v>2024-11-04T07:01:58.019</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:G11"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:G17"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>